<commit_message>
finished draft of full example
</commit_message>
<xml_diff>
--- a/full-example.xlsx
+++ b/full-example.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="232">
   <si>
     <t xml:space="preserve">Introduction</t>
   </si>
@@ -406,28 +406,76 @@
       <t xml:space="preserve">knitr</t>
     </r>
     <r>
-      <t xml:space="preserve">. For example: $\pi = 3.1415927$.</t>
+      <t xml:space="preserve">. For example: 𝜋= 3.1415927.</t>
     </r>
   </si>
   <si>
     <t xml:space="preserve">Executing Code Chunks</t>
   </si>
   <si>
-    <t xml:space="preserve">echo, include, </t>
-  </si>
-  <si>
-    <t xml:space="preserve">error warnings messages</t>
-  </si>
-  <si>
-    <t xml:space="preserve">rendering data.frames, vector, prints, </t>
-  </si>
-  <si>
-    <t xml:space="preserve">plots (fig.width, ...)</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Customizing </t>
-    </r>
+    <t xml:space="preserve">1``</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Evaluation Parameters</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The following code chunk is not echoed:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">## [1] "Not echoed"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The following code chunk is not included:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">print("Not included")</t>
+  </si>
+  <si>
+    <t xml:space="preserve">## [1] "Not included"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The following code chunk is not evaluated:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">print("Not evaluated")</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Errors, Warnings and Messages</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Errors, warning and messages are rendered with special styles.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"># This is an error</t>
+  </si>
+  <si>
+    <t xml:space="preserve">log("a string")</t>
+  </si>
+  <si>
+    <t xml:space="preserve">## Error in log("a string"): non-numeric argument to mathematical function</t>
+  </si>
+  <si>
+    <t xml:space="preserve"># This is a warning</t>
+  </si>
+  <si>
+    <t xml:space="preserve">log(-1)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">## Warning in log(-1): NaNs produced</t>
+  </si>
+  <si>
+    <t xml:space="preserve"># This is a message</t>
+  </si>
+  <si>
+    <t xml:space="preserve">message("my message")</t>
+  </si>
+  <si>
+    <t xml:space="preserve">## my message</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rendering Basic Types</t>
+  </si>
+  <si>
     <r>
       <rPr>
         <b/>
@@ -437,12 +485,575 @@
       </rPr>
       <t xml:space="preserve">knitxl</t>
     </r>
-  </si>
-  <si>
-    <t xml:space="preserve">Styling</t>
+    <r>
+      <t xml:space="preserve"> knows how to render a few basic types.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">Data Frames</t>
+    </r>
+    <r>
+      <t xml:space="preserve">:</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">head(iris)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sepal.Length</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sepal.Width</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Petal.Length</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Petal.Width</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Species</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">setosa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">Vectors</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Named vector:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">islands[1:10]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Africa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Antarctica</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Asia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Australia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Axel Heiberg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Baffin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Banks</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Borneo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Britain</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Celebes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Unnamed vector:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">letters[1:10]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">a</t>
+  </si>
+  <si>
+    <t xml:space="preserve">b</t>
+  </si>
+  <si>
+    <t xml:space="preserve">c</t>
+  </si>
+  <si>
+    <t xml:space="preserve">d</t>
+  </si>
+  <si>
+    <t xml:space="preserve">e</t>
+  </si>
+  <si>
+    <t xml:space="preserve">f</t>
+  </si>
+  <si>
+    <t xml:space="preserve">g</t>
+  </si>
+  <si>
+    <t xml:space="preserve">h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">i</t>
+  </si>
+  <si>
+    <t xml:space="preserve">j</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">By default other types of object are rendered as a text via the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FF395392"/>
+        <rFont val="Courier New"/>
+      </rPr>
+      <t xml:space="preserve">print</t>
+    </r>
+    <r>
+      <t xml:space="preserve"> function:</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">fit &lt;- lm(mpg ~ cyl, data = mtcars)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">summary(fit)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">## </t>
+  </si>
+  <si>
+    <t xml:space="preserve">## Call:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">## lm(formula = mpg ~ cyl, data = mtcars)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">## Residuals:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">##     Min      1Q  Median      3Q     Max </t>
+  </si>
+  <si>
+    <t xml:space="preserve">## -4.9814 -2.1185  0.2217  1.0717  7.5186 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">## Coefficients:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">##             Estimate Std. Error t value Pr(&gt;|t|)    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">## (Intercept)  37.8846     2.0738   18.27  &lt; 2e-16 ***</t>
+  </si>
+  <si>
+    <t xml:space="preserve">## cyl          -2.8758     0.3224   -8.92 6.11e-10 ***</t>
+  </si>
+  <si>
+    <t xml:space="preserve">## ---</t>
+  </si>
+  <si>
+    <t xml:space="preserve">## Signif. codes:  0 '***' 0.001 '**' 0.01 '*' 0.05 '.' 0.1 ' ' 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">## Residual standard error: 3.206 on 30 degrees of freedom</t>
+  </si>
+  <si>
+    <t xml:space="preserve">## Multiple R-squared:  0.7262,	Adjusted R-squared:  0.7171 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">## F-statistic: 79.56 on 1 and 30 DF,  p-value: 6.113e-10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Plots</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Currently the only chunk options recognized are </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FF395392"/>
+        <rFont val="Courier New"/>
+      </rPr>
+      <t xml:space="preserve">fig.width</t>
+    </r>
+    <r>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FF395392"/>
+        <rFont val="Courier New"/>
+      </rPr>
+      <t xml:space="preserve">fig.height</t>
+    </r>
+    <r>
+      <t xml:space="preserve"> and</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FF395392"/>
+        <rFont val="Courier New"/>
+      </rPr>
+      <t xml:space="preserve">dpi</t>
+    </r>
+    <r>
+      <t xml:space="preserve">:</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">with(mtcars, {</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  plot(mpg~hp, pch=20, col='darkgray')</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  lines(lowess(hp, mpg))</t>
+  </si>
+  <si>
+    <t xml:space="preserve">})</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Customizing </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FF395392"/>
+        <rFont val="Courier New"/>
+      </rPr>
+      <t xml:space="preserve">knitxl</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">Custom renderers</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Developers can implement custom rendering function for specific classes.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">For examples, for the class </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FF395392"/>
+        <rFont val="Courier New"/>
+      </rPr>
+      <t xml:space="preserve">lm</t>
+    </r>
+    <r>
+      <t xml:space="preserve">, we might want to display specific information</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">about the linear model in the output Excel file:</t>
+  </si>
+  <si>
+    <t xml:space="preserve"># This is the custom renderer for `lm` objects.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"># It will display the coefficients of the linear model</t>
+  </si>
+  <si>
+    <t xml:space="preserve"># in a table.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">xl_renderer.lm &lt;- function(x, options) {</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  summary(x)$coefficients %&gt;%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    as.data.frame() %&gt;%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    knitxl:::new_knitxl_output_data_frame()</t>
+  </si>
+  <si>
+    <t xml:space="preserve">}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">registerS3method("xl_renderer", "lm", xl_renderer.lm)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lm_object &lt;- lm(mpg ~ cyl, data = mtcars)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lm_object</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Estimate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Std. Error</t>
+  </si>
+  <si>
+    <t xml:space="preserve">t value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pr(&gt;|t|)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(Intercept)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cyl</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Custom styles</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Style customization is not yet supported but is being considered for the next</t>
+  </si>
+  <si>
+    <t xml:space="preserve">release. Under the hood, the default style is implemented in this way:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">kxl_style(xl.gridlines = FALSE,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">xl.fontName = "Calibri",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">xl.fontSize = 11,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">xl.rowHeight = 12.75,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">xl.text.h1.fontName = "Calibri Light (Headings)",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">xl.text.h1.fontSize = 18,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">xl.text.h1.fontColour = "#475368",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">xl.text.h2.fontName = "Calibri (Body)",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">xl.text.h2.fontSize = 15,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">xl.text.h2.fontColour = "#475368",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">xl.text.h2.textDecoration = "bold",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">xl.text.h2.border = "bottom",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">xl.text.h2.borderStyle = "thick",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">xl.text.h2.borderColour = "#4F71BE",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">xl.text.h3.fontName = "Calibri (Body)",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">xl.text.h3.fontSize = 13,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">xl.text.h3.fontColour = "#475368",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">xl.text.h3.textDecoration = "bold",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">xl.text.h3.border = "bottom",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">xl.text.h3.borderStyle = "thick",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">xl.text.h3.borderColour = "#A6B7DE",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">xl.text.h4.fontName = "Calibri (Body)",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">xl.text.h4.fontSize = 11,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">xl.text.h4.fontColour = "#475368",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">xl.text.h4.textDecoration = "bold",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">xl.text.h4.border = "bottom",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">xl.text.h4.borderStyle = "medium",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">xl.text.h4.borderColour = "#A6B7DE",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">xl.text.h5.fontName = "Calibri (Body)",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">xl.text.h5.fontSize = 11,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">xl.text.h5.fontColour = "#475368",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">xl.text.h5.textDecoration = "bold",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">xl.text.h6.fontName = "Calibri (Body)",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">xl.text.h6.fontSize = 11,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">xl.text.h6.fontColour = "#475368",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">xl.text.h6.textDecoration = "italic",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">xl.text.hrule.border = "top",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">xl.text.hrule.borderStyle = "thick",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">xl.text.hrule.borderColour = "black",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">xl.text.blockquote.textDecoration = "italic",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">xl.text.blockquote.indent = 1,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">xl.text.blockquote.fontColour = "#7F7F7F",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">xl.text.error.fontColour = "red",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">xl.text.error.textDecoration = "bold",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">xl.text.warning.fontColour = "orange",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">xl.text.warning.textDecoration = "bold",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">xl.text.message.fontColour = "blue",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">xl.text.message.textDecoration = "italic",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">xl.text.output.fontColour = "grey",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">xl.text.output.fontName = "Courier New",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">xl.text.output.textDecoration = "italic",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">xl.text.source.fontName = "Courier New",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">xl.vector.numFmt = "GENERAL",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">xl.vector.direction = "vertical",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">xl.vector.names.textDecoration = "bold",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">xl.vector.names.border = "right",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">xl.vector.names.borderStyle = "thin",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">xl.vector.names.borderColour = "black",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">xl.table.numFmt = "GENERAL",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">xl.table.direction = "vertical",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">xl.table.maxrows = 50,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">xl.table.colNames = TRUE,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">xl.table.rowNames = TRUE,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">xl.table.header.border = "bottom",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">xl.table.header.textDecoration = "bold",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">xl.table.header.halign = "center",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">xl.table.rownames.fontColour = "grey",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">xl.table.rownames.border = "right")</t>
   </si>
 </sst>
 </file>
@@ -450,7 +1061,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="0"/>
-  <fonts count="10">
+  <fonts count="16">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -509,6 +1120,41 @@
       <name val="Calibri"/>
       <i/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFBEBEBE"/>
+      <name val="Courier New"/>
+      <i/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <b/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFFA500"/>
+      <name val="Calibri"/>
+      <b/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <i/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <b/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFBEBEBE"/>
+      <name val="Calibri"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -518,7 +1164,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -546,11 +1192,21 @@
         <color rgb="FFA6B7DE"/>
       </bottom>
     </border>
+    <border>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+    </border>
+    <border>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -565,6 +1221,15 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -583,6 +1248,41 @@
       <xdr:rowOff xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">0</xdr:rowOff>
     </xdr:from>
     <xdr:ext xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" cx="9194800" cy="7124700"/>
+    <xdr:pic xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+      <xdr:nvPicPr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+        <xdr:cNvPr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" id="1" name="Picture 1"/>
+        <xdr:cNvPicPr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+          <a:picLocks xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+        </a:blip>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <xdr:oneCellAnchor xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+    <xdr:from xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+      <xdr:col xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">1</xdr:col>
+      <xdr:colOff xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">0</xdr:colOff>
+      <xdr:row xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">127</xdr:row>
+      <xdr:rowOff xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" cx="9144000" cy="9144000"/>
     <xdr:pic xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
       <xdr:nvPicPr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
         <xdr:cNvPr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" id="1" name="Picture 1"/>
@@ -1213,34 +1913,575 @@
         <v>51</v>
       </c>
     </row>
+    <row r="7">
+      <c r="A7" s="4" t="s">
+        <v>52</v>
+      </c>
+    </row>
     <row r="8">
-      <c r="A8" s="4" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="2" t="s">
+      <c r="A8" s="2" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="12">
-      <c r="A12" s="2" t="s">
+    <row r="9">
+      <c r="A9" s="6" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="14">
-      <c r="A14" s="2" t="s">
+    <row r="11">
+      <c r="A11" s="2" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="16">
-      <c r="A16" s="2" t="s">
+    <row r="13">
+      <c r="A13" s="12" t="s">
         <v>56</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="12" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="6" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="3" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="3" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="13" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="3" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="3" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="14" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="2" t="e">
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="3" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="3" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="15" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="6" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="2" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" s="3" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="s">
+        <v>12</v>
+      </c>
+      <c r="B54" s="16" t="s">
+        <v>77</v>
+      </c>
+      <c r="C54" s="16" t="s">
+        <v>78</v>
+      </c>
+      <c r="D54" s="16" t="s">
+        <v>79</v>
+      </c>
+      <c r="E54" s="16" t="s">
+        <v>80</v>
+      </c>
+      <c r="F54" s="16" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" s="17" t="s">
+        <v>82</v>
+      </c>
+      <c r="B55" s="2" t="n">
+        <v>5.1</v>
+      </c>
+      <c r="C55" s="2" t="n">
+        <v>3.5</v>
+      </c>
+      <c r="D55" s="2" t="n">
+        <v>1.4</v>
+      </c>
+      <c r="E55" s="2" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="F55" s="2" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" s="17" t="s">
+        <v>84</v>
+      </c>
+      <c r="B56" s="2" t="n">
+        <v>4.9</v>
+      </c>
+      <c r="C56" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="D56" s="2" t="n">
+        <v>1.4</v>
+      </c>
+      <c r="E56" s="2" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="F56" s="2" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" s="17" t="s">
+        <v>85</v>
+      </c>
+      <c r="B57" s="2" t="n">
+        <v>4.7</v>
+      </c>
+      <c r="C57" s="2" t="n">
+        <v>3.2</v>
+      </c>
+      <c r="D57" s="2" t="n">
+        <v>1.3</v>
+      </c>
+      <c r="E57" s="2" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="F57" s="2" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" s="17" t="s">
+        <v>86</v>
+      </c>
+      <c r="B58" s="2" t="n">
+        <v>4.6</v>
+      </c>
+      <c r="C58" s="2" t="n">
+        <v>3.1</v>
+      </c>
+      <c r="D58" s="2" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="E58" s="2" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="F58" s="2" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" s="17" t="s">
+        <v>87</v>
+      </c>
+      <c r="B59" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="C59" s="2" t="n">
+        <v>3.6</v>
+      </c>
+      <c r="D59" s="2" t="n">
+        <v>1.4</v>
+      </c>
+      <c r="E59" s="2" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="F59" s="2" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" s="17" t="s">
+        <v>88</v>
+      </c>
+      <c r="B60" s="2" t="n">
+        <v>5.4</v>
+      </c>
+      <c r="C60" s="2" t="n">
+        <v>3.9</v>
+      </c>
+      <c r="D60" s="2" t="n">
+        <v>1.7</v>
+      </c>
+      <c r="E60" s="2" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="F60" s="2" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" s="2" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" s="2" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" s="3" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" s="18" t="s">
+        <v>92</v>
+      </c>
+      <c r="B68" s="2" t="n">
+        <v>11506</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" s="18" t="s">
+        <v>93</v>
+      </c>
+      <c r="B69" s="2" t="n">
+        <v>5500</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" s="18" t="s">
+        <v>94</v>
+      </c>
+      <c r="B70" s="2" t="n">
+        <v>16988</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" s="18" t="s">
+        <v>95</v>
+      </c>
+      <c r="B71" s="2" t="n">
+        <v>2968</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" s="18" t="s">
+        <v>96</v>
+      </c>
+      <c r="B72" s="2" t="n">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" s="18" t="s">
+        <v>97</v>
+      </c>
+      <c r="B73" s="2" t="n">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" s="18" t="s">
+        <v>98</v>
+      </c>
+      <c r="B74" s="2" t="n">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" s="18" t="s">
+        <v>99</v>
+      </c>
+      <c r="B75" s="2" t="n">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" s="18" t="s">
+        <v>100</v>
+      </c>
+      <c r="B76" s="2" t="n">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" s="18" t="s">
+        <v>101</v>
+      </c>
+      <c r="B77" s="2" t="n">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" s="2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" s="3" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" s="2" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" s="2" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" s="2" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" s="2" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" s="2" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" s="2" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" s="2" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" s="2" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" s="2" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" s="2" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" s="2" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" s="3" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" s="3" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" s="12" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" s="12" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" s="12" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" s="12" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" s="12" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" s="12" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" s="12" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" s="12" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" s="12" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" s="12" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" s="12" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" s="12" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" s="12" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" s="12" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" s="12" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" s="12" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" s="12" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" s="12" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" s="6" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" s="2" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" s="2" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" s="3" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" s="3" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" s="3" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" s="3" t="s">
+        <v>138</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1254,17 +2495,568 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>57</v>
+        <v>139</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="4" t="s">
-        <v>58</v>
+        <v>140</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="2" t="s">
+        <v>141</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="4" t="s">
-        <v>59</v>
+      <c r="A6" s="2" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="2" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="3" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="3" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="3" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="3" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="3" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="3" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="3" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="3" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="3" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="3" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="3" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="s">
+        <v>12</v>
+      </c>
+      <c r="B23" s="16" t="s">
+        <v>155</v>
+      </c>
+      <c r="C23" s="16" t="s">
+        <v>156</v>
+      </c>
+      <c r="D23" s="16" t="s">
+        <v>157</v>
+      </c>
+      <c r="E23" s="16" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="17" t="s">
+        <v>159</v>
+      </c>
+      <c r="B24" s="2" t="n">
+        <v>37.8845764854614</v>
+      </c>
+      <c r="C24" s="2" t="n">
+        <v>2.07384360552423</v>
+      </c>
+      <c r="D24" s="2" t="n">
+        <v>18.2678078445963</v>
+      </c>
+      <c r="E24" s="2" t="n">
+        <v>0.00000000000000000836915530493018</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="17" t="s">
+        <v>160</v>
+      </c>
+      <c r="B25" s="2" t="n">
+        <v>-2.87579013906447</v>
+      </c>
+      <c r="C25" s="2" t="n">
+        <v>0.322408882659104</v>
+      </c>
+      <c r="D25" s="2" t="n">
+        <v>-8.91969884745751</v>
+      </c>
+      <c r="E25" s="2" t="n">
+        <v>0.000000000611268714258103</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="4" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="2" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="2" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="3" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="3" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="3" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="3" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="3" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="3" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="3" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="3" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="3" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="3" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="3" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="3" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="3" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="3" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="3" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="3" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="3" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="3" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" s="3" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" s="3" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" s="3" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" s="3" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" s="3" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" s="3" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" s="3" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" s="3" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" s="3" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" s="3" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" s="3" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" s="3" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" s="3" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" s="3" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" s="3" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" s="3" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" s="3" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" s="3" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" s="3" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" s="3" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" s="3" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" s="3" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" s="3" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" s="3" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" s="3" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" s="3" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" s="3" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" s="3" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" s="3" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" s="3" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" s="3" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" s="3" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" s="3" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" s="3" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" s="3" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" s="3" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" s="3" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" s="3" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" s="3" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" s="3" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" s="3" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" s="3" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" s="3" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" s="3" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" s="3" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" s="3" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" s="3" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" s="3" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" s="3" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" s="3" t="s">
+        <v>231</v>
       </c>
     </row>
   </sheetData>

</xml_diff>